<commit_message>
Added Research and Development team
</commit_message>
<xml_diff>
--- a/2ndyear.xlsx
+++ b/2ndyear.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="132">
   <si>
     <t>Rohan Sharma</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>LinkedIn</t>
-  </si>
-  <si>
-    <t>Sila Puja</t>
   </si>
   <si>
     <t>Zadziya Pattnaik</t>
@@ -824,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,10 +862,10 @@
         <v>52</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -880,10 +877,10 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -897,7 +894,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -911,10 +908,10 @@
         <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -928,10 +925,10 @@
         <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -950,10 +947,10 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -967,7 +964,7 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -981,10 +978,10 @@
         <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -998,7 +995,7 @@
         <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1012,10 +1009,10 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1034,7 +1031,7 @@
         <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1048,7 +1045,7 @@
         <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1062,7 +1059,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1076,10 +1073,10 @@
         <v>64</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1093,10 +1090,10 @@
         <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1110,7 +1107,7 @@
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1122,10 +1119,10 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1139,10 +1136,10 @@
         <v>67</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1156,10 +1153,10 @@
         <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,7 +1181,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,7 +1193,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1210,10 +1207,10 @@
         <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1227,10 +1224,10 @@
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1242,7 +1239,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1256,7 +1253,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1270,7 +1267,7 @@
         <v>74</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,10 +1281,10 @@
         <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1304,13 +1301,13 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1321,10 +1318,10 @@
         <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1336,13 +1333,13 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -1353,29 +1350,29 @@
         <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>